<commit_message>
Edited the map to include a down door. Added to the OurTest file
</commit_message>
<xml_diff>
--- a/MapOfCampusCLUE.xlsx
+++ b/MapOfCampusCLUE.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\datwh\Documents\College\Sophmore\Spring\Soft E\Clue noncode files\Clue\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\datwh\Documents\College\Sophmore\Spring\Soft E\Labs\Clue\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39049FBA-DE93-41CA-9076-479183A09E09}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F9F889F-0FC2-41D0-9467-5CA75DDC8985}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FEEFAB7E-8D71-41ED-9D3E-D1228D75F521}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1404" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="702" uniqueCount="39">
   <si>
     <t>X</t>
   </si>
@@ -148,6 +148,9 @@
   </si>
   <si>
     <t>W&lt;</t>
+  </si>
+  <si>
+    <t>Wv</t>
   </si>
 </sst>
 </file>
@@ -565,7 +568,7 @@
   <dimension ref="A1:AB27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2325,7 +2328,7 @@
         <v>6</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="G21" s="2" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
Finished writing jUnits, need to fix errors
</commit_message>
<xml_diff>
--- a/MapOfCampusCLUE.xlsx
+++ b/MapOfCampusCLUE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\datwh\Documents\College\Sophmore\Spring\Soft E\Labs\Clue\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F9F889F-0FC2-41D0-9467-5CA75DDC8985}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6303AA9A-CF13-4491-BB18-C8B417708EAD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FEEFAB7E-8D71-41ED-9D3E-D1228D75F521}"/>
   </bookViews>
@@ -568,7 +568,7 @@
   <dimension ref="A1:AB27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+      <selection activeCell="AJ12" sqref="AJ12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1788,7 +1788,7 @@
       <c r="Z14" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AA14" s="1" t="s">
+      <c r="AA14" s="9" t="s">
         <v>34</v>
       </c>
       <c r="AB14" s="1" t="s">
@@ -1871,7 +1871,7 @@
       <c r="Y15" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="Z15" s="1" t="s">
+      <c r="Z15" s="9" t="s">
         <v>35</v>
       </c>
       <c r="AA15" s="1" t="s">

</xml_diff>

<commit_message>
Editied our jUnit test file that contained incorrect information
</commit_message>
<xml_diff>
--- a/MapOfCampusCLUE.xlsx
+++ b/MapOfCampusCLUE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\datwh\Documents\College\Sophmore\Spring\Soft E\Labs\Clue\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6303AA9A-CF13-4491-BB18-C8B417708EAD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D936A98B-B635-4040-B388-5CB80F961FE7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FEEFAB7E-8D71-41ED-9D3E-D1228D75F521}"/>
   </bookViews>
@@ -568,7 +568,7 @@
   <dimension ref="A1:AB27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="AJ12" sqref="AJ12"/>
+      <selection activeCell="AI16" sqref="AI16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1112,7 +1112,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>1</v>

</xml_diff>

<commit_message>
Edited location of strings for room labels
</commit_message>
<xml_diff>
--- a/MapOfCampusCLUE.xlsx
+++ b/MapOfCampusCLUE.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\datwh\Documents\College\Sophmore\Spring\Soft E\Labs\Clue\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D936A98B-B635-4040-B388-5CB80F961FE7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{951A8F44-3A96-4007-BE0A-79B88B3743CB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FEEFAB7E-8D71-41ED-9D3E-D1228D75F521}"/>
   </bookViews>
@@ -568,7 +568,7 @@
   <dimension ref="A1:AB27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="AI16" sqref="AI16"/>
+      <selection activeCell="AD25" sqref="AD25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1871,11 +1871,11 @@
       <c r="Y15" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="Z15" s="9" t="s">
+      <c r="Z15" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA15" s="9" t="s">
         <v>35</v>
-      </c>
-      <c r="AA15" s="1" t="s">
-        <v>33</v>
       </c>
       <c r="AB15" s="1" t="s">
         <v>33</v>
@@ -2499,8 +2499,8 @@
       <c r="E23" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F23" s="8" t="s">
-        <v>9</v>
+      <c r="F23" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="G23" s="2" t="s">
         <v>7</v>
@@ -2579,8 +2579,8 @@
       <c r="C24" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D24" s="2" t="s">
-        <v>7</v>
+      <c r="D24" s="8" t="s">
+        <v>9</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>7</v>

</xml_diff>